<commit_message>
updated gdp eleasticity to take out ind (already include covid in bifubc)
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
+++ b/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\ctrl-settings\EoSEUwGDPiR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\Canada\canada-eps\InputData\ctrl-settings\EoSEUwGDPiR\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6D7994-6C11-44CA-B737-552735E498C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <sheet name="EIA" sheetId="8" r:id="rId5"/>
     <sheet name="EoSEUwGDPiR" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,6 +31,8 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1050,7 +1053,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -1454,24 +1457,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.59765625" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
@@ -1479,161 +1482,161 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
     </row>
-    <row r="18" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
     </row>
-    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
     </row>
-    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29"/>
     </row>
-    <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B30"/>
     </row>
-    <row r="31" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>329</v>
       </c>
       <c r="B31"/>
     </row>
-    <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>330</v>
       </c>
       <c r="B32"/>
     </row>
-    <row r="33" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>328</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1641,7 +1644,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -1651,25 +1654,25 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.59765625" customWidth="1"/>
-    <col min="2" max="2" width="27.3984375" customWidth="1"/>
-    <col min="3" max="3" width="17.265625" customWidth="1"/>
-    <col min="4" max="4" width="16.73046875" customWidth="1"/>
-    <col min="5" max="5" width="19.265625" customWidth="1"/>
-    <col min="6" max="6" width="11.265625" customWidth="1"/>
-    <col min="7" max="7" width="87.73046875" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="87.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>331</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>321</v>
       </c>
@@ -1677,12 +1680,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>5</v>
       </c>
@@ -1695,7 +1698,7 @@
         <v>-3.382663847780127E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>57</v>
       </c>
@@ -1708,7 +1711,7 @@
         <v>-6.9450186027283992E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>56</v>
       </c>
@@ -1721,12 +1724,12 @@
         <v>-0.11888111888111895</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>5</v>
       </c>
@@ -1739,7 +1742,7 @@
         <v>3.2890132960111965E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>57</v>
       </c>
@@ -1750,7 +1753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>56</v>
       </c>
@@ -1763,12 +1766,12 @@
         <v>-4.3572984749455312E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>5</v>
       </c>
@@ -1781,7 +1784,7 @@
         <v>-5.9778597785977862E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>57</v>
       </c>
@@ -1793,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>56</v>
       </c>
@@ -1806,18 +1809,18 @@
         <v>-7.3995771670190377E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="23"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>2019</v>
       </c>
@@ -1825,7 +1828,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>29</v>
       </c>
@@ -1838,7 +1841,7 @@
         <v>18411</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <f>-(1-C20/B20)</f>
         <v>-5.3321678321678334E-2</v>
@@ -1848,12 +1851,12 @@
       </c>
       <c r="C22" s="15"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>7</v>
       </c>
@@ -1873,7 +1876,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -1899,11 +1902,11 @@
       </c>
       <c r="G26" s="24"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F27" s="12"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>9</v>
       </c>
@@ -1936,19 +1939,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AG181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:AG181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.53125" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -2049,7 +2052,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>61</v>
       </c>
@@ -2150,7 +2153,7 @@
         <v>421200000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>62</v>
       </c>
@@ -2251,7 +2254,7 @@
         <v>1069000000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -2352,7 +2355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>64</v>
       </c>
@@ -2453,7 +2456,7 @@
         <v>147800000000000</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>65</v>
       </c>
@@ -2554,7 +2557,7 @@
         <v>1153000000000000</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>66</v>
       </c>
@@ -2655,7 +2658,7 @@
         <v>1963000000000000</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -2756,7 +2759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -2857,7 +2860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -2958,7 +2961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -3059,7 +3062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -3160,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -3261,7 +3264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>73</v>
       </c>
@@ -3362,7 +3365,7 @@
         <v>2494000000000000</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>74</v>
       </c>
@@ -3463,7 +3466,7 @@
         <v>44000000000000</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -3564,7 +3567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -3665,7 +3668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>77</v>
       </c>
@@ -3766,7 +3769,7 @@
         <v>1082000000000000</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>78</v>
       </c>
@@ -3867,7 +3870,7 @@
         <v>162800000000000</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>79</v>
       </c>
@@ -3968,7 +3971,7 @@
         <v>151900000000000</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -4069,7 +4072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>81</v>
       </c>
@@ -4170,7 +4173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>82</v>
       </c>
@@ -4271,7 +4274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>83</v>
       </c>
@@ -4372,7 +4375,7 @@
         <v>18570000000000</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>84</v>
       </c>
@@ -4473,7 +4476,7 @@
         <v>5059000000000</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>85</v>
       </c>
@@ -4574,7 +4577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -4675,7 +4678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -4776,7 +4779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>88</v>
       </c>
@@ -4877,7 +4880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -4978,7 +4981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>90</v>
       </c>
@@ -5079,7 +5082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
         <v>91</v>
       </c>
@@ -5180,7 +5183,7 @@
         <v>244300000000000</v>
       </c>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>92</v>
       </c>
@@ -5281,7 +5284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>93</v>
       </c>
@@ -5382,7 +5385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>94</v>
       </c>
@@ -5483,7 +5486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -5584,7 +5587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -5685,7 +5688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -5786,7 +5789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>98</v>
       </c>
@@ -5887,7 +5890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>99</v>
       </c>
@@ -5988,7 +5991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>100</v>
       </c>
@@ -6089,7 +6092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>101</v>
       </c>
@@ -6190,7 +6193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>102</v>
       </c>
@@ -6291,7 +6294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>103</v>
       </c>
@@ -6392,7 +6395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>104</v>
       </c>
@@ -6493,7 +6496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>105</v>
       </c>
@@ -6594,7 +6597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>106</v>
       </c>
@@ -6695,7 +6698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>107</v>
       </c>
@@ -6796,7 +6799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>108</v>
       </c>
@@ -6897,7 +6900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
         <v>109</v>
       </c>
@@ -6998,7 +7001,7 @@
         <v>151200000000000</v>
       </c>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>110</v>
       </c>
@@ -7099,7 +7102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>111</v>
       </c>
@@ -7200,7 +7203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>112</v>
       </c>
@@ -7301,7 +7304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="s">
         <v>113</v>
       </c>
@@ -7402,7 +7405,7 @@
         <v>31710000000000</v>
       </c>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
         <v>114</v>
       </c>
@@ -7503,7 +7506,7 @@
         <v>91150000000000</v>
       </c>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>115</v>
       </c>
@@ -7604,7 +7607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>116</v>
       </c>
@@ -7705,7 +7708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>117</v>
       </c>
@@ -7806,7 +7809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -7907,7 +7910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>119</v>
       </c>
@@ -8008,7 +8011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>120</v>
       </c>
@@ -8109,7 +8112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="s">
         <v>121</v>
       </c>
@@ -8210,7 +8213,7 @@
         <v>104500000000000</v>
       </c>
     </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A63" s="22" t="s">
         <v>122</v>
       </c>
@@ -8311,7 +8314,7 @@
         <v>265200000000000</v>
       </c>
     </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>123</v>
       </c>
@@ -8412,7 +8415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A65" s="22" t="s">
         <v>124</v>
       </c>
@@ -8513,7 +8516,7 @@
         <v>36670000000000</v>
       </c>
     </row>
-    <row r="66" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A66" s="22" t="s">
         <v>125</v>
       </c>
@@ -8614,7 +8617,7 @@
         <v>286000000000000</v>
       </c>
     </row>
-    <row r="67" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A67" s="22" t="s">
         <v>126</v>
       </c>
@@ -8715,7 +8718,7 @@
         <v>487200000000000</v>
       </c>
     </row>
-    <row r="68" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>127</v>
       </c>
@@ -8816,7 +8819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>128</v>
       </c>
@@ -8917,7 +8920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>129</v>
       </c>
@@ -9018,7 +9021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>130</v>
       </c>
@@ -9119,7 +9122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>131</v>
       </c>
@@ -9220,7 +9223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>132</v>
       </c>
@@ -9321,7 +9324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A74" s="22" t="s">
         <v>133</v>
       </c>
@@ -9422,7 +9425,7 @@
         <v>618900000000000</v>
       </c>
     </row>
-    <row r="75" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A75" s="22" t="s">
         <v>134</v>
       </c>
@@ -9523,7 +9526,7 @@
         <v>10920000000000</v>
       </c>
     </row>
-    <row r="76" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>135</v>
       </c>
@@ -9624,7 +9627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>136</v>
       </c>
@@ -9725,7 +9728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A78" s="22" t="s">
         <v>137</v>
       </c>
@@ -9826,7 +9829,7 @@
         <v>268400000000000</v>
       </c>
     </row>
-    <row r="79" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A79" s="22" t="s">
         <v>138</v>
       </c>
@@ -9927,7 +9930,7 @@
         <v>40390000000000</v>
       </c>
     </row>
-    <row r="80" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A80" s="22" t="s">
         <v>139</v>
       </c>
@@ -10028,7 +10031,7 @@
         <v>37700000000000</v>
       </c>
     </row>
-    <row r="81" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>140</v>
       </c>
@@ -10129,7 +10132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>141</v>
       </c>
@@ -10230,7 +10233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>142</v>
       </c>
@@ -10331,7 +10334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A84" s="22" t="s">
         <v>143</v>
       </c>
@@ -10432,7 +10435,7 @@
         <v>4609000000000</v>
       </c>
     </row>
-    <row r="85" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A85" s="22" t="s">
         <v>144</v>
       </c>
@@ -10533,7 +10536,7 @@
         <v>1256000000000</v>
       </c>
     </row>
-    <row r="86" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>145</v>
       </c>
@@ -10634,7 +10637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>146</v>
       </c>
@@ -10735,7 +10738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>147</v>
       </c>
@@ -10836,7 +10839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>148</v>
       </c>
@@ -10937,7 +10940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>149</v>
       </c>
@@ -11038,7 +11041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>150</v>
       </c>
@@ -11139,7 +11142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A92" s="22" t="s">
         <v>151</v>
       </c>
@@ -11240,7 +11243,7 @@
         <v>60630000000000</v>
       </c>
     </row>
-    <row r="93" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>152</v>
       </c>
@@ -11341,7 +11344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>153</v>
       </c>
@@ -11442,7 +11445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>154</v>
       </c>
@@ -11543,7 +11546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>155</v>
       </c>
@@ -11644,7 +11647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>156</v>
       </c>
@@ -11745,7 +11748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>157</v>
       </c>
@@ -11846,7 +11849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>158</v>
       </c>
@@ -11947,7 +11950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>159</v>
       </c>
@@ -12048,7 +12051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>160</v>
       </c>
@@ -12149,7 +12152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>161</v>
       </c>
@@ -12250,7 +12253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>162</v>
       </c>
@@ -12351,7 +12354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>163</v>
       </c>
@@ -12452,7 +12455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>164</v>
       </c>
@@ -12553,7 +12556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>165</v>
       </c>
@@ -12654,7 +12657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>166</v>
       </c>
@@ -12755,7 +12758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>167</v>
       </c>
@@ -12856,7 +12859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>168</v>
       </c>
@@ -12957,7 +12960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A110" s="22" t="s">
         <v>169</v>
       </c>
@@ -13058,7 +13061,7 @@
         <v>37530000000000</v>
       </c>
     </row>
-    <row r="111" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>170</v>
       </c>
@@ -13159,7 +13162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>171</v>
       </c>
@@ -13260,7 +13263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>172</v>
       </c>
@@ -13361,7 +13364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A114" s="22" t="s">
         <v>173</v>
       </c>
@@ -13462,7 +13465,7 @@
         <v>7869000000000</v>
       </c>
     </row>
-    <row r="115" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A115" s="22" t="s">
         <v>174</v>
       </c>
@@ -13563,7 +13566,7 @@
         <v>22620000000000</v>
       </c>
     </row>
-    <row r="116" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>175</v>
       </c>
@@ -13664,7 +13667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>176</v>
       </c>
@@ -13765,7 +13768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>177</v>
       </c>
@@ -13866,7 +13869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>178</v>
       </c>
@@ -13967,7 +13970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>179</v>
       </c>
@@ -14068,7 +14071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>180</v>
       </c>
@@ -14169,7 +14172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A122" s="22" t="s">
         <v>181</v>
       </c>
@@ -14270,7 +14273,7 @@
         <v>88660000000000</v>
       </c>
     </row>
-    <row r="123" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A123" s="22" t="s">
         <v>182</v>
       </c>
@@ -14371,7 +14374,7 @@
         <v>1045000000000000</v>
       </c>
     </row>
-    <row r="124" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>183</v>
       </c>
@@ -14472,7 +14475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A125" s="22" t="s">
         <v>184</v>
       </c>
@@ -14573,7 +14576,7 @@
         <v>335000000000000</v>
       </c>
     </row>
-    <row r="126" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A126" s="22" t="s">
         <v>185</v>
       </c>
@@ -14674,7 +14677,7 @@
         <v>868000000000000</v>
       </c>
     </row>
-    <row r="127" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A127" s="22" t="s">
         <v>186</v>
       </c>
@@ -14775,7 +14778,7 @@
         <v>3561000000000000</v>
       </c>
     </row>
-    <row r="128" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>187</v>
       </c>
@@ -14876,7 +14879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>188</v>
       </c>
@@ -14977,7 +14980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>189</v>
       </c>
@@ -15078,7 +15081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>190</v>
       </c>
@@ -15179,7 +15182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>191</v>
       </c>
@@ -15280,7 +15283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A133" s="22" t="s">
         <v>192</v>
       </c>
@@ -15381,7 +15384,7 @@
         <v>24420000000000</v>
       </c>
     </row>
-    <row r="134" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A134" s="22" t="s">
         <v>193</v>
       </c>
@@ -15482,7 +15485,7 @@
         <v>1828000000000000</v>
       </c>
     </row>
-    <row r="135" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A135" s="22" t="s">
         <v>194</v>
       </c>
@@ -15583,7 +15586,7 @@
         <v>23090000000000</v>
       </c>
     </row>
-    <row r="136" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>195</v>
       </c>
@@ -15684,7 +15687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>196</v>
       </c>
@@ -15785,7 +15788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A138" s="22" t="s">
         <v>197</v>
       </c>
@@ -15886,7 +15889,7 @@
         <v>1258000000000000</v>
       </c>
     </row>
-    <row r="139" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A139" s="22" t="s">
         <v>198</v>
       </c>
@@ -15987,7 +15990,7 @@
         <v>777700000000000</v>
       </c>
     </row>
-    <row r="140" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A140" s="22" t="s">
         <v>199</v>
       </c>
@@ -16088,7 +16091,7 @@
         <v>163200000000000</v>
       </c>
     </row>
-    <row r="141" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>200</v>
       </c>
@@ -16189,7 +16192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>201</v>
       </c>
@@ -16290,7 +16293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>202</v>
       </c>
@@ -16391,7 +16394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A144" s="22" t="s">
         <v>203</v>
       </c>
@@ -16492,7 +16495,7 @@
         <v>5642000000000</v>
       </c>
     </row>
-    <row r="145" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A145" s="22" t="s">
         <v>204</v>
       </c>
@@ -16593,7 +16596,7 @@
         <v>116500000000000</v>
       </c>
     </row>
-    <row r="146" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A146" s="22" t="s">
         <v>205</v>
       </c>
@@ -16694,7 +16697,7 @@
         <v>313500000000000</v>
       </c>
     </row>
-    <row r="147" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>206</v>
       </c>
@@ -16795,7 +16798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>207</v>
       </c>
@@ -16896,7 +16899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>208</v>
       </c>
@@ -16997,7 +17000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>209</v>
       </c>
@@ -17098,7 +17101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>210</v>
       </c>
@@ -17199,7 +17202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>211</v>
       </c>
@@ -17300,7 +17303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>212</v>
       </c>
@@ -17401,7 +17404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>213</v>
       </c>
@@ -17502,7 +17505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>214</v>
       </c>
@@ -17603,7 +17606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>215</v>
       </c>
@@ -17704,7 +17707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>216</v>
       </c>
@@ -17805,7 +17808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>217</v>
       </c>
@@ -17906,7 +17909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>218</v>
       </c>
@@ -18007,7 +18010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>219</v>
       </c>
@@ -18108,7 +18111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>220</v>
       </c>
@@ -18209,7 +18212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>221</v>
       </c>
@@ -18310,7 +18313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>222</v>
       </c>
@@ -18411,7 +18414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>223</v>
       </c>
@@ -18512,7 +18515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>224</v>
       </c>
@@ -18613,7 +18616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>225</v>
       </c>
@@ -18714,7 +18717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>226</v>
       </c>
@@ -18815,7 +18818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>227</v>
       </c>
@@ -18916,7 +18919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>228</v>
       </c>
@@ -19017,7 +19020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A170" s="22" t="s">
         <v>229</v>
       </c>
@@ -19118,7 +19121,7 @@
         <v>335300000000000</v>
       </c>
     </row>
-    <row r="171" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>230</v>
       </c>
@@ -19219,7 +19222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>231</v>
       </c>
@@ -19320,7 +19323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>232</v>
       </c>
@@ -19421,7 +19424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A174" s="22" t="s">
         <v>233</v>
       </c>
@@ -19522,7 +19525,7 @@
         <v>11590000000000</v>
       </c>
     </row>
-    <row r="175" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A175" s="22" t="s">
         <v>234</v>
       </c>
@@ -19623,7 +19626,7 @@
         <v>239300000000000</v>
       </c>
     </row>
-    <row r="176" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>235</v>
       </c>
@@ -19724,7 +19727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>236</v>
       </c>
@@ -19825,7 +19828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>237</v>
       </c>
@@ -19926,7 +19929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>238</v>
       </c>
@@ -20027,7 +20030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>239</v>
       </c>
@@ -20128,7 +20131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>240</v>
       </c>
@@ -20235,16 +20238,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AG81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:AG81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -20345,7 +20348,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>241</v>
       </c>
@@ -20446,7 +20449,7 @@
         <v>43400000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>242</v>
       </c>
@@ -20547,7 +20550,7 @@
         <v>106900000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>243</v>
       </c>
@@ -20648,7 +20651,7 @@
         <v>47200000000000</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>244</v>
       </c>
@@ -20749,7 +20752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>245</v>
       </c>
@@ -20850,7 +20853,7 @@
         <v>48300000000000</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>246</v>
       </c>
@@ -20951,7 +20954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>247</v>
       </c>
@@ -21052,7 +21055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>248</v>
       </c>
@@ -21153,7 +21156,7 @@
         <v>14500000000000</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>249</v>
       </c>
@@ -21254,7 +21257,7 @@
         <v>200000000000</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>250</v>
       </c>
@@ -21355,7 +21358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>251</v>
       </c>
@@ -21456,7 +21459,7 @@
         <v>196500000000000</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>252</v>
       </c>
@@ -21557,7 +21560,7 @@
         <v>32600000000000</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>253</v>
       </c>
@@ -21658,7 +21661,7 @@
         <v>5321000000000000</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>254</v>
       </c>
@@ -21759,7 +21762,7 @@
         <v>932100000000000</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>255</v>
       </c>
@@ -21860,7 +21863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>256</v>
       </c>
@@ -21961,7 +21964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>257</v>
       </c>
@@ -22062,7 +22065,7 @@
         <v>3.94654E+16</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>258</v>
       </c>
@@ -22163,7 +22166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>259</v>
       </c>
@@ -22264,7 +22267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>260</v>
       </c>
@@ -22365,7 +22368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>261</v>
       </c>
@@ -22466,7 +22469,7 @@
         <v>203800000000000</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>262</v>
       </c>
@@ -22567,7 +22570,7 @@
         <v>471400000000000</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>263</v>
       </c>
@@ -22668,7 +22671,7 @@
         <v>372200000000000</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>264</v>
       </c>
@@ -22769,7 +22772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>265</v>
       </c>
@@ -22870,7 +22873,7 @@
         <v>1500000000000</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>266</v>
       </c>
@@ -22971,7 +22974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>267</v>
       </c>
@@ -23072,7 +23075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>268</v>
       </c>
@@ -23173,7 +23176,7 @@
         <v>23500000000000</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
         <v>269</v>
       </c>
@@ -23274,7 +23277,7 @@
         <v>100000000000</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>270</v>
       </c>
@@ -23375,7 +23378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
         <v>271</v>
       </c>
@@ -23476,7 +23479,7 @@
         <v>509100000000000</v>
       </c>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
         <v>272</v>
       </c>
@@ -23577,7 +23580,7 @@
         <v>56200000000000</v>
       </c>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
         <v>273</v>
       </c>
@@ -23678,7 +23681,7 @@
         <v>5621000000000000</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>274</v>
       </c>
@@ -23779,7 +23782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
         <v>275</v>
       </c>
@@ -23880,7 +23883,7 @@
         <v>132300000000000</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>276</v>
       </c>
@@ -23981,7 +23984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>277</v>
       </c>
@@ -24082,7 +24085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
         <v>278</v>
       </c>
@@ -24183,7 +24186,7 @@
         <v>156300000000000</v>
       </c>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
         <v>279</v>
       </c>
@@ -24284,7 +24287,7 @@
         <v>6015600000000000</v>
       </c>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>280</v>
       </c>
@@ -24385,7 +24388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
         <v>281</v>
       </c>
@@ -24486,7 +24489,7 @@
         <v>84010000000000</v>
       </c>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
         <v>282</v>
       </c>
@@ -24587,7 +24590,7 @@
         <v>98200000000000</v>
       </c>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>283</v>
       </c>
@@ -24688,7 +24691,7 @@
         <v>70220000000000</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>284</v>
       </c>
@@ -24789,7 +24792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
         <v>285</v>
       </c>
@@ -24890,7 +24893,7 @@
         <v>45450000000000</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>286</v>
       </c>
@@ -24991,7 +24994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>287</v>
       </c>
@@ -25092,7 +25095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
         <v>288</v>
       </c>
@@ -25193,7 +25196,7 @@
         <v>15807100000000</v>
       </c>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>289</v>
       </c>
@@ -25294,7 +25297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>290</v>
       </c>
@@ -25395,7 +25398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
         <v>291</v>
       </c>
@@ -25496,7 +25499,7 @@
         <v>263000000000000</v>
       </c>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>292</v>
       </c>
@@ -25597,7 +25600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>293</v>
       </c>
@@ -25698,7 +25701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>294</v>
       </c>
@@ -25799,7 +25802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>295</v>
       </c>
@@ -25900,7 +25903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>296</v>
       </c>
@@ -26001,7 +26004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>297</v>
       </c>
@@ -26102,7 +26105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>298</v>
       </c>
@@ -26203,7 +26206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>299</v>
       </c>
@@ -26304,7 +26307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>300</v>
       </c>
@@ -26405,7 +26408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="s">
         <v>301</v>
       </c>
@@ -26506,7 +26509,7 @@
         <v>355700000000000</v>
       </c>
     </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>302</v>
       </c>
@@ -26607,7 +26610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A64" s="22" t="s">
         <v>303</v>
       </c>
@@ -26708,7 +26711,7 @@
         <v>218800000000000</v>
       </c>
     </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>304</v>
       </c>
@@ -26809,7 +26812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A66" s="22" t="s">
         <v>305</v>
       </c>
@@ -26910,7 +26913,7 @@
         <v>693000000000000</v>
       </c>
     </row>
-    <row r="67" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>306</v>
       </c>
@@ -27011,7 +27014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>307</v>
       </c>
@@ -27112,7 +27115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A69" s="22" t="s">
         <v>308</v>
       </c>
@@ -27213,7 +27216,7 @@
         <v>94200000000000</v>
       </c>
     </row>
-    <row r="70" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A70" s="22" t="s">
         <v>309</v>
       </c>
@@ -27314,7 +27317,7 @@
         <v>113500000000000</v>
       </c>
     </row>
-    <row r="71" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>310</v>
       </c>
@@ -27415,7 +27418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A72" s="22" t="s">
         <v>311</v>
       </c>
@@ -27516,7 +27519,7 @@
         <v>2392000000000000</v>
       </c>
     </row>
-    <row r="73" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A73" s="22" t="s">
         <v>312</v>
       </c>
@@ -27617,7 +27620,7 @@
         <v>167300000000000</v>
       </c>
     </row>
-    <row r="74" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A74" s="22" t="s">
         <v>313</v>
       </c>
@@ -27718,7 +27721,7 @@
         <v>3816000000000000</v>
       </c>
     </row>
-    <row r="75" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>314</v>
       </c>
@@ -27819,7 +27822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A76" s="22" t="s">
         <v>315</v>
       </c>
@@ -27920,7 +27923,7 @@
         <v>2975000000000000</v>
       </c>
     </row>
-    <row r="77" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>316</v>
       </c>
@@ -28021,7 +28024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>317</v>
       </c>
@@ -28122,7 +28125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A79" s="22" t="s">
         <v>318</v>
       </c>
@@ -28223,7 +28226,7 @@
         <v>241162000000000</v>
       </c>
     </row>
-    <row r="80" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A80" s="22" t="s">
         <v>319</v>
       </c>
@@ -28324,7 +28327,7 @@
         <v>120600000000000</v>
       </c>
     </row>
-    <row r="81" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>320</v>
       </c>
@@ -28431,20 +28434,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.59765625" customWidth="1"/>
-    <col min="6" max="6" width="16.86328125" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>33</v>
       </c>
@@ -28458,7 +28461,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>322</v>
       </c>
@@ -28484,7 +28487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -28512,7 +28515,7 @@
         <v>-4.3572984749455312E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -28540,7 +28543,7 @@
         <v>-7.3995771670190377E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -28568,7 +28571,7 @@
         <v>-6.9450186027283992E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -28583,7 +28586,7 @@
         <v>-1.8532818532818532E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -28597,7 +28600,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
         <v>43</v>
       </c>
@@ -28620,7 +28623,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>31</v>
       </c>
@@ -28648,7 +28651,7 @@
         <v>0.28571428571428581</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>55</v>
       </c>
@@ -28663,7 +28666,7 @@
         <v>-0.11888111888111895</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -28684,20 +28687,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.1328125" customWidth="1"/>
+    <col min="1" max="1" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -28705,7 +28710,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -28714,16 +28719,15 @@
         <v>2.5234299846339887</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="14">
-        <f>Calculations!F28</f>
-        <v>0.34756630166466224</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -28732,7 +28736,7 @@
         <v>0.12159295854427969</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -28741,16 +28745,15 @@
         <v>1.2332258830457008</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="7">
-        <f>Calculations!D28</f>
-        <v>1.8462747301314177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -28758,7 +28761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -28766,7 +28769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>

</xml_diff>